<commit_message>
selection file : add readAntares
</commit_message>
<xml_diff>
--- a/inst/application/www/readAntares_selection.xlsx
+++ b/inst/application/www/readAntares_selection.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Datastorm\Documents\git\antaresVizMedTSO\inst\application\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3058CF91-F11D-4764-9754-669B7BB77D25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2C2601-B562-46C9-818D-D421DEB229B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="681" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="681" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Noeuds" sheetId="1" r:id="rId1"/>
-    <sheet name="Liens" sheetId="3" r:id="rId2"/>
+    <sheet name="Areas" sheetId="1" r:id="rId1"/>
+    <sheet name="Links" sheetId="3" r:id="rId2"/>
     <sheet name="Clusters" sheetId="4" r:id="rId3"/>
     <sheet name="Districts" sheetId="5" r:id="rId4"/>
-    <sheet name="Autres paramètres" sheetId="6" r:id="rId5"/>
+    <sheet name="readAntares" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="111">
   <si>
     <t>AL00</t>
   </si>
@@ -175,27 +175,18 @@
     <t>misc</t>
   </si>
   <si>
-    <t>vide</t>
-  </si>
-  <si>
     <t>thermalAvailability</t>
   </si>
   <si>
     <t>hydroStorage</t>
   </si>
   <si>
-    <t xml:space="preserve">hydroStorageMaxPower  </t>
-  </si>
-  <si>
     <t>reserve</t>
   </si>
   <si>
     <t>linkCapacity</t>
   </si>
   <si>
-    <t>selected</t>
-  </si>
-  <si>
     <t>mustRun</t>
   </si>
   <si>
@@ -205,24 +196,6 @@
     <t>timeStep</t>
   </si>
   <si>
-    <t>Hourly</t>
-  </si>
-  <si>
-    <t>mcYears selection</t>
-  </si>
-  <si>
-    <t>custom</t>
-  </si>
-  <si>
-    <t>Choose mcYears</t>
-  </si>
-  <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t>readAntares parameters</t>
-  </si>
-  <si>
     <t>CO2 EMIS.</t>
   </si>
   <si>
@@ -337,12 +310,6 @@
     <t>HURDLE COST</t>
   </si>
   <si>
-    <t>Remove virtual Areas</t>
-  </si>
-  <si>
-    <t>enabled</t>
-  </si>
-  <si>
     <t>storageFlexibility</t>
   </si>
   <si>
@@ -353,15 +320,74 @@
   </si>
   <si>
     <t>newCols</t>
+  </si>
+  <si>
+    <t>parameters</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>0 disabled - 1 enabled</t>
+  </si>
+  <si>
+    <t>hourly, daily, weekly, monthly, annual</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>mcYears</t>
+  </si>
+  <si>
+    <t>removeVirtualAreas</t>
+  </si>
+  <si>
+    <t>names of the virtual storage/flexibility areas</t>
+  </si>
+  <si>
+    <t>name of the columns to import</t>
+  </si>
+  <si>
+    <t>names of the virtual production areas, or empty / NULL / NA</t>
+  </si>
+  <si>
+    <t>a number or synthetic, or empty / NULL / NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydroStorageMaxPower </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -387,8 +413,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,190 +703,190 @@
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -870,15 +901,15 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="8" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -894,7 +925,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="19.25" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
@@ -902,152 +933,152 @@
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1063,7 +1094,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
@@ -1073,52 +1104,52 @@
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1130,371 +1161,426 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="34.125" customWidth="1"/>
+    <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.75" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>52</v>
       </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="18" spans="2:2">
+      <c r="B18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B14">
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="B49" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+      <c r="C50" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+      <c r="B51" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="B53" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+      <c r="C57" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+      <c r="B58" s="3">
+        <v>0</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+      <c r="B59" s="3">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>104</v>
-      </c>
-      <c r="B59" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>105</v>
-      </c>
-      <c r="B66" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>106</v>
-      </c>
-      <c r="B68" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>107</v>
-      </c>
-      <c r="B69" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1504,12 +1590,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1704,15 +1787,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33171608-4890-453C-9EEB-B02C4FA97B47}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf004ee6-088f-48ca-90d3-808610fc13fe"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1737,18 +1832,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33171608-4890-453C-9EEB-B02C4FA97B47}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cf004ee6-088f-48ca-90d3-808610fc13fe"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
udpate default selection file
</commit_message>
<xml_diff>
--- a/inst/application/www/readAntares_selection.xlsx
+++ b/inst/application/www/readAntares_selection.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Datastorm\Documents\git\antaresVizMedTSO\inst\application\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bueemm\Documents\2 - MedTSO\WG ESS\Data and Tools\Market Tools\antaresViz for Med-TSO\Specifications\General parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2C2601-B562-46C9-818D-D421DEB229B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="681" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="681" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="104">
   <si>
     <t>AL00</t>
   </si>
@@ -157,12 +156,6 @@
     <t>0_TURB_Daily</t>
   </si>
   <si>
-    <t>0_PUMP_Weekly</t>
-  </si>
-  <si>
-    <t>0_TURB_Weekly</t>
-  </si>
-  <si>
     <t>1_PUMP_MAROC</t>
   </si>
   <si>
@@ -280,36 +273,15 @@
     <t>NP COST</t>
   </si>
   <si>
-    <t>NODU</t>
-  </si>
-  <si>
     <t>FLOW LIN.</t>
   </si>
   <si>
-    <t>UCAP LIN.</t>
-  </si>
-  <si>
-    <t>FLOW QUAD.</t>
-  </si>
-  <si>
-    <t>CONG. FEE (ALG.)</t>
-  </si>
-  <si>
-    <t>CONG. FEE (ABS.)</t>
-  </si>
-  <si>
-    <t>MARG. COST</t>
-  </si>
-  <si>
     <t>CONG. PROB +</t>
   </si>
   <si>
     <t>CONG. PROB -</t>
   </si>
   <si>
-    <t>HURDLE COST</t>
-  </si>
-  <si>
     <t>storageFlexibility</t>
   </si>
   <si>
@@ -362,13 +334,19 @@
   </si>
   <si>
     <t xml:space="preserve">hydroStorageMaxPower </t>
+  </si>
+  <si>
+    <t>1_PUMP_Weekly</t>
+  </si>
+  <si>
+    <t>1_TURB_Weekly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -699,196 +677,196 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -897,21 +875,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="8.375" customWidth="1"/>
+    <col min="1" max="8" width="8.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -920,165 +898,165 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="19.19921875" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="21.625" customWidth="1"/>
+    <col min="7" max="7" width="21.59765625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1089,67 +1067,67 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.09765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1160,427 +1138,392 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="A37" sqref="A37:XFD38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.125" customWidth="1"/>
+    <col min="1" max="1" width="34.09765625" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.75" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.69921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" s="3" t="s">
+      <c r="C47" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" s="3" t="s">
+      <c r="C50" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" s="3" t="s">
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" s="3" t="s">
+      <c r="B52" s="3">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="B49" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>105</v>
-      </c>
-      <c r="B50" s="3">
-        <v>1</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>93</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="B52" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="B53" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="B54" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="B55" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="B56" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>95</v>
-      </c>
-      <c r="B58" s="3">
-        <v>0</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" s="3">
-        <v>0</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1590,14 +1533,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100677214EBD8584B4CA94D8F15CA747198" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="86616bf523250a85ec9dc85aa805df82">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="702dd7b0-da09-4dc6-8207-dc22fe143878" xmlns:ns3="cf004ee6-088f-48ca-90d3-808610fc13fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35c77b5dcc3153392ae36517355ea8fc" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100677214EBD8584B4CA94D8F15CA747198" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="22d1c103c0d1d6b790ff68146c39531f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="702dd7b0-da09-4dc6-8207-dc22fe143878" xmlns:ns3="cf004ee6-088f-48ca-90d3-808610fc13fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6379b4b0374c01e5098f6864432e8956" ns2:_="" ns3:_="">
     <xsd:import namespace="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
     <xsd:import namespace="cf004ee6-088f-48ca-90d3-808610fc13fe"/>
     <xsd:element name="properties">
@@ -1614,6 +1560,8 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1652,6 +1600,16 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -1787,54 +1745,36 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57F8658F-C32B-479A-8CBE-5C448D1FF341}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33171608-4890-453C-9EEB-B02C4FA97B47}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="cf004ee6-088f-48ca-90d3-808610fc13fe"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FDCB3A6-2382-4223-AC6F-C692503F6F99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
-    <ds:schemaRef ds:uri="cf004ee6-088f-48ca-90d3-808610fc13fe"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
generate & download selection file
</commit_message>
<xml_diff>
--- a/inst/application/www/readAntares_selection.xlsx
+++ b/inst/application/www/readAntares_selection.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bueemm\Documents\2 - MedTSO\WG ESS\Data and Tools\Market Tools\antaresViz for Med-TSO\Specifications\General parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Datastorm\Documents\git\antaresVizMedTSO\inst\application\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E916FE21-E1DA-4ABD-BC49-E1A092809C2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="681" activeTab="4"/>
+    <workbookView xWindow="1065" yWindow="3300" windowWidth="15360" windowHeight="9360" tabRatio="681" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>AL00</t>
   </si>
@@ -327,12 +328,6 @@
     <t>name of the columns to import</t>
   </si>
   <si>
-    <t>names of the virtual production areas, or empty / NULL / NA</t>
-  </si>
-  <si>
-    <t>a number or synthetic, or empty / NULL / NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">hydroStorageMaxPower </t>
   </si>
   <si>
@@ -340,13 +335,16 @@
   </si>
   <si>
     <t>1_TURB_Weekly</t>
+  </si>
+  <si>
+    <t>one or more numbers (separated by ;) or synthetic, or empty / NULL / NA. Multiple years : 1;2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -677,194 +675,194 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -875,19 +873,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="8" width="8.3984375" customWidth="1"/>
+    <col min="1" max="8" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -898,165 +896,165 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="19.19921875" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="21.59765625" customWidth="1"/>
+    <col min="7" max="7" width="21.625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1067,67 +1065,67 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1138,21 +1136,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD38"/>
+      <selection activeCell="C1" sqref="C1:C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="34.09765625" customWidth="1"/>
+    <col min="1" max="1" width="34.125" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.69921875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.75" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -1163,7 +1161,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1174,7 +1172,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1185,7 +1183,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1196,9 +1194,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1207,7 +1205,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1218,7 +1216,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1229,7 +1227,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1240,7 +1238,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1251,7 +1249,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1262,7 +1260,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -1270,10 +1268,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -1284,227 +1282,212 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="B14" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2">
       <c r="B17" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2">
       <c r="B18" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2">
       <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2">
       <c r="B20" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2">
       <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2">
       <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2">
       <c r="B23" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2">
       <c r="B24" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2">
       <c r="B25" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2">
       <c r="B26" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2">
       <c r="B27" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2">
       <c r="B28" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2">
       <c r="B29" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2">
       <c r="B30" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2">
       <c r="B31" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2">
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="B33" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="B34" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="B35" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="B36" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="B37" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="B38" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="B39" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="B40" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="B41" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="B42" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>96</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3">
       <c r="B45" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3">
       <c r="B46" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3">
       <c r="B47" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3">
       <c r="B48" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3">
       <c r="B49" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>85</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -1512,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -1523,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1533,15 +1516,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100677214EBD8584B4CA94D8F15CA747198" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="22d1c103c0d1d6b790ff68146c39531f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="702dd7b0-da09-4dc6-8207-dc22fe143878" xmlns:ns3="cf004ee6-088f-48ca-90d3-808610fc13fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6379b4b0374c01e5098f6864432e8956" ns2:_="" ns3:_="">
     <xsd:import namespace="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
@@ -1744,6 +1718,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1751,15 +1734,30 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57F8658F-C32B-479A-8CBE-5C448D1FF341}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
+    <ds:schemaRef ds:uri="cf004ee6-088f-48ca-90d3-808610fc13fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57F8658F-C32B-479A-8CBE-5C448D1FF341}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
new storageFlexibility + multiple rm virtual area + V8.1 clusterRes
</commit_message>
<xml_diff>
--- a/inst/application/www/readAntares_selection.xlsx
+++ b/inst/application/www/readAntares_selection.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Datastorm\Documents\git\antaresVizMedTSO\inst\application\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenoitThieurmel\Documents\git\antaresVizMedTSO\inst\application\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E916FE21-E1DA-4ABD-BC49-E1A092809C2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5051E145-50F2-400B-9548-F9817E9D7D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="3300" windowWidth="15360" windowHeight="9360" tabRatio="681" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="681" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" r:id="rId1"/>
     <sheet name="Links" sheetId="3" r:id="rId2"/>
     <sheet name="Clusters" sheetId="4" r:id="rId3"/>
-    <sheet name="Districts" sheetId="5" r:id="rId4"/>
-    <sheet name="readAntares" sheetId="6" r:id="rId5"/>
+    <sheet name="ClustersRes" sheetId="7" r:id="rId4"/>
+    <sheet name="Districts" sheetId="5" r:id="rId5"/>
+    <sheet name="readAntares" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -682,9 +683,9 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -880,9 +881,9 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="8" width="8.375" customWidth="1"/>
+    <col min="1" max="8" width="8.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -901,11 +902,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="19.19921875" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="21.625" customWidth="1"/>
+    <col min="7" max="7" width="21.59765625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1065,18 +1066,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E601A4-0020-4D6E-AE6F-BECDAD258160}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.09765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1135,19 +1150,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="34.125" customWidth="1"/>
+    <col min="1" max="1" width="34.09765625" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.75" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.69921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1516,6 +1531,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100677214EBD8584B4CA94D8F15CA747198" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="22d1c103c0d1d6b790ff68146c39531f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="702dd7b0-da09-4dc6-8207-dc22fe143878" xmlns:ns3="cf004ee6-088f-48ca-90d3-808610fc13fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6379b4b0374c01e5098f6864432e8956" ns2:_="" ns3:_="">
     <xsd:import namespace="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
@@ -1718,22 +1748,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33171608-4890-453C-9EEB-B02C4FA97B47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf004ee6-088f-48ca-90d3-808610fc13fe"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57F8658F-C32B-479A-8CBE-5C448D1FF341}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1750,29 +1790,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33171608-4890-453C-9EEB-B02C4FA97B47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cf004ee6-088f-48ca-90d3-808610fc13fe"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
read / write xlsx selection with new storage
</commit_message>
<xml_diff>
--- a/inst/application/www/readAntares_selection.xlsx
+++ b/inst/application/www/readAntares_selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenoitThieurmel\Documents\git\antaresVizMedTSO\inst\application\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5051E145-50F2-400B-9548-F9817E9D7D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CB9A48-F4DE-4FD3-8DFD-4708956B7CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="681" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="681" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="138">
   <si>
     <t>AL00</t>
   </si>
@@ -284,9 +284,6 @@
     <t>CONG. PROB -</t>
   </si>
   <si>
-    <t>storageFlexibility</t>
-  </si>
-  <si>
     <t>production</t>
   </si>
   <si>
@@ -323,9 +320,6 @@
     <t>removeVirtualAreas</t>
   </si>
   <si>
-    <t>names of the virtual storage/flexibility areas</t>
-  </si>
-  <si>
     <t>name of the columns to import</t>
   </si>
   <si>
@@ -339,6 +333,117 @@
   </si>
   <si>
     <t>one or more numbers (separated by ;) or synthetic, or empty / NULL / NA. Multiple years : 1;2</t>
+  </si>
+  <si>
+    <t>names of the virtual productions areas</t>
+  </si>
+  <si>
+    <t>names of the virtual storage/flexibility areas PSP</t>
+  </si>
+  <si>
+    <t>Hydro Storage (PSP_Closed)</t>
+  </si>
+  <si>
+    <t>storageFlexibility (PSP)</t>
+  </si>
+  <si>
+    <t>names of the virtual hydro storage areas PSP_Closed</t>
+  </si>
+  <si>
+    <t>Battery Storage (BATT)</t>
+  </si>
+  <si>
+    <t>Demand Side (DSR)</t>
+  </si>
+  <si>
+    <t>Electric Vehicle (EV)</t>
+  </si>
+  <si>
+    <t>Power-to-gas (P2G)</t>
+  </si>
+  <si>
+    <t>Hydrogen (H2)</t>
+  </si>
+  <si>
+    <t>names of the virtual battery storage areas BATT</t>
+  </si>
+  <si>
+    <t>names of the virtual demand side areas DSR</t>
+  </si>
+  <si>
+    <t>names of the virtual electric vehicle areas EV</t>
+  </si>
+  <si>
+    <t>names of the virtual power to gas areas P2G</t>
+  </si>
+  <si>
+    <t>names of the virtual hydrogen areas H2</t>
+  </si>
+  <si>
+    <t>removeVirtualAreas_2</t>
+  </si>
+  <si>
+    <t>storageFlexibility (PSP)_2</t>
+  </si>
+  <si>
+    <t>Hydro Storage (PSP_Closed)_2</t>
+  </si>
+  <si>
+    <t>Battery Storage (BATT)_2</t>
+  </si>
+  <si>
+    <t>Demand Side (DSR)_2</t>
+  </si>
+  <si>
+    <t>Electric Vehicle (EV)_2</t>
+  </si>
+  <si>
+    <t>Power-to-gas (P2G)_2</t>
+  </si>
+  <si>
+    <t>Hydrogen (H2)_2</t>
+  </si>
+  <si>
+    <t>production_2</t>
+  </si>
+  <si>
+    <t>reassignCost_2</t>
+  </si>
+  <si>
+    <t>newCols_2</t>
+  </si>
+  <si>
+    <t>removeVirtualAreas_3</t>
+  </si>
+  <si>
+    <t>storageFlexibility (PSP)_3</t>
+  </si>
+  <si>
+    <t>Hydro Storage (PSP_Closed)_3</t>
+  </si>
+  <si>
+    <t>Battery Storage (BATT)_3</t>
+  </si>
+  <si>
+    <t>Demand Side (DSR)_3</t>
+  </si>
+  <si>
+    <t>Electric Vehicle (EV)_3</t>
+  </si>
+  <si>
+    <t>Power-to-gas (P2G)_3</t>
+  </si>
+  <si>
+    <t>Hydrogen (H2)_3</t>
+  </si>
+  <si>
+    <t>production_3</t>
+  </si>
+  <si>
+    <t>reassignCost_3</t>
+  </si>
+  <si>
+    <t>newCols_3</t>
   </si>
 </sst>
 </file>
@@ -850,12 +955,12 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:1">
@@ -1069,7 +1174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E601A4-0020-4D6E-AE6F-BECDAD258160}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -1152,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
@@ -1167,13 +1272,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1184,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1195,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1206,18 +1311,18 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1228,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1239,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1250,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1261,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1269,32 +1374,32 @@
         <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1449,20 +1554,25 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
       </c>
+      <c r="C43" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="3" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="3" t="s">
@@ -1472,13 +1582,13 @@
     </row>
     <row r="46" spans="1:3">
       <c r="B46" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C47" s="2"/>
     </row>
@@ -1496,32 +1606,274 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" s="3">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>87</v>
-      </c>
-      <c r="B52" s="3">
+        <v>107</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="3">
         <v>0</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>97</v>
+      <c r="C57" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="3">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="3">
+        <v>0</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="3">
+        <v>0</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="3">
+        <v>0</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>127</v>
+      </c>
+      <c r="B70" s="3">
+        <v>0</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>132</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>133</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>134</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>136</v>
+      </c>
+      <c r="B79" s="3">
+        <v>0</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>137</v>
+      </c>
+      <c r="B80" s="3">
+        <v>0</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1537,15 +1889,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100677214EBD8584B4CA94D8F15CA747198" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="22d1c103c0d1d6b790ff68146c39531f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="702dd7b0-da09-4dc6-8207-dc22fe143878" xmlns:ns3="cf004ee6-088f-48ca-90d3-808610fc13fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6379b4b0374c01e5098f6864432e8956" ns2:_="" ns3:_="">
     <xsd:import namespace="702dd7b0-da09-4dc6-8207-dc22fe143878"/>
@@ -1748,6 +2091,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33171608-4890-453C-9EEB-B02C4FA97B47}">
   <ds:schemaRefs>
@@ -1766,14 +2118,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57F8658F-C32B-479A-8CBE-5C448D1FF341}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1790,4 +2134,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CA4496-1FEF-4232-B64E-75D1ECB1B703}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>